<commit_message>
Enhance the pure data-driven.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excel/testdata.xlsx
+++ b/src/test/resources/testdata/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bselvaraju\Documents\ui\GWS UI\ui_testframework\src\test\resources\testdata\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pon Vignesh.K\OneDrive\src\test\resources\testdata\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80618826-3A03-4510-B194-151F84E9307F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>testdescription</t>
   </si>
@@ -164,12 +165,18 @@
   </si>
   <si>
     <t>To verify that a user can send a message from the Bridge portal to OP.</t>
+  </si>
+  <si>
+    <t>loginLogoutTest</t>
+  </si>
+  <si>
+    <t>QA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,11 +488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +526,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -561,11 +568,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +580,7 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -601,10 +608,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -843,15 +850,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="33" customWidth="1"/>
     <col min="5" max="5" width="72.7109375" customWidth="1"/>
     <col min="6" max="6" width="62.7109375" customWidth="1"/>
     <col min="7" max="7" width="55.140625" customWidth="1"/>

</xml_diff>